<commit_message>
Added draft 1.3.0 documentation
Not really - is currently copy of 1.2.0 docs...
</commit_message>
<xml_diff>
--- a/documentation/Defects and Enhancements.xlsx
+++ b/documentation/Defects and Enhancements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16ecbb52d5e766a3/Documents/TechStuff/Projects/Enlarger_Timer/FADU_Timer/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bob\OneDrive\Documents\TechStuff\Projects\Enlarger_Timer\FADU_Timer\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="8_{3CBD49A9-EBAC-4436-B860-85F4D7170538}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{FD27CD33-2055-4781-A7F6-9C6485676C97}"/>
+  <xr:revisionPtr revIDLastSave="199" documentId="8_{3CBD49A9-EBAC-4436-B860-85F4D7170538}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{38577ADB-93B4-4E26-B95F-AAA2327A2817}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{736E6442-F76E-41A5-9606-E17F3A3051F3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>Status</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>To be updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -696,7 +699,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,7 +951,9 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>

</xml_diff>

<commit_message>
Update Defects and Enhancements.xlsx
</commit_message>
<xml_diff>
--- a/documentation/Defects and Enhancements.xlsx
+++ b/documentation/Defects and Enhancements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bob\OneDrive\Documents\TechStuff\Projects\Enlarger_Timer\FADU_Timer\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="199" documentId="8_{3CBD49A9-EBAC-4436-B860-85F4D7170538}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{38577ADB-93B4-4E26-B95F-AAA2327A2817}"/>
+  <xr:revisionPtr revIDLastSave="218" documentId="8_{3CBD49A9-EBAC-4436-B860-85F4D7170538}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{30400351-4450-42CC-B274-723D92DDA3F7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{736E6442-F76E-41A5-9606-E17F3A3051F3}"/>
+    <workbookView xWindow="2895" yWindow="2820" windowWidth="24705" windowHeight="12015" xr2:uid="{736E6442-F76E-41A5-9606-E17F3A3051F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="44">
   <si>
     <t>Status</t>
   </si>
@@ -147,7 +147,22 @@
     <t>To be updated</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>CONT mode</t>
+  </si>
+  <si>
+    <t>FIX IT!</t>
+  </si>
+  <si>
+    <t>Reverted code changes that caused the issue.  I am an idiot</t>
+  </si>
+  <si>
+    <t>Timing runnning slow per strip</t>
+  </si>
+  <si>
+    <t>FIxing 7 above broke [RST] in STRIPS mode</t>
+  </si>
+  <si>
+    <t>Restore functionality</t>
   </si>
 </sst>
 </file>
@@ -698,9 +713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871DEB98-E520-4C60-BE88-D7878B15EB24}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -946,36 +959,64 @@
       </c>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="H10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="F11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Latest Defects & Enhancements doc
</commit_message>
<xml_diff>
--- a/documentation/Defects and Enhancements.xlsx
+++ b/documentation/Defects and Enhancements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bob\OneDrive\Documents\TechStuff\Projects\Enlarger_Timer\FADU_Timer\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="222" documentId="8_{3CBD49A9-EBAC-4436-B860-85F4D7170538}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{FCEBDBAB-7D54-4CF8-A46C-E6239534102C}"/>
+  <xr:revisionPtr revIDLastSave="239" documentId="8_{3CBD49A9-EBAC-4436-B860-85F4D7170538}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{2A079F58-97CF-43B2-939A-A46AAF3BCFB4}"/>
   <bookViews>
     <workbookView xWindow="2895" yWindow="2820" windowWidth="24705" windowHeight="12015" xr2:uid="{736E6442-F76E-41A5-9606-E17F3A3051F3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
   <si>
     <t>Status</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Lowered end-beep and incresed strip-end warning beep frequencies. Tick shorter and colume increased to fit other sounds better.  Trimmed all silence from samples.</t>
   </si>
   <si>
-    <t>N/S</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -166,6 +163,21 @@
   </si>
   <si>
     <t>Functionality restored.</t>
+  </si>
+  <si>
+    <t>CONT mode with delay</t>
+  </si>
+  <si>
+    <t>seems the two CONT modes do not like each other…  With/without delay = mutually exclusive.</t>
+  </si>
+  <si>
+    <t>Same as 1.  Fixing it broke Counin = 0 mode!</t>
+  </si>
+  <si>
+    <t>Redesign.  Now three Strips Modes to avoiud confusion when using Delay to define which CONT mode we are in.  MAN: manual = stops at the end of each strip;  STEP: Delay at end of each strip;  CONT : does not stop - beeps at 0.5s defore the end of each strip.</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -213,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -226,9 +238,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -383,8 +392,8 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFFF8080"/>
       <color rgb="FFFF4040"/>
-      <color rgb="FFFF8080"/>
     </mruColors>
   </colors>
   <extLst>
@@ -716,7 +725,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871DEB98-E520-4C60-BE88-D7878B15EB24}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -779,7 +790,7 @@
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -802,35 +813,35 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <f>A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -934,7 +945,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -942,23 +953,23 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="J9" s="2"/>
     </row>
@@ -983,16 +994,16 @@
         <v>9</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" s="4" t="s">
+      <c r="J10" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1016,35 +1027,53 @@
         <v>9</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    </row>
+    <row r="12" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>

</xml_diff>